<commit_message>
se modificaron las consultas para condicionarlas al periodo actual
</commit_message>
<xml_diff>
--- a/Asignacion Tutorias LAM.xlsx
+++ b/Asignacion Tutorias LAM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>REGISTRO DE REPORTES DE TUTORÍAS SEMESTRE feb2019-agos2019</t>
   </si>
@@ -51,10 +51,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>2017030557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARANGO SUMANO GUADALUPE </t>
+    <t>2018010071</t>
+  </si>
+  <si>
+    <t>REYES  MOJICA DELFINO MISAEL</t>
   </si>
   <si>
     <t>LAM</t>
@@ -66,147 +66,66 @@
     <t>2</t>
   </si>
   <si>
-    <t>2018010005</t>
-  </si>
-  <si>
-    <t>GARCIA CRUZ JAVIER LEOPOLDO</t>
+    <t>2018010072</t>
+  </si>
+  <si>
+    <t>GARCIA MARTINEZ DIEGO</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>2018010006</t>
-  </si>
-  <si>
-    <t>GARCIA GARCIA ESTEFANIA</t>
+    <t>2018010083</t>
+  </si>
+  <si>
+    <t>AGUILLON CHAVEZ JESUS</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>2018010007</t>
-  </si>
-  <si>
-    <t>SANTIAGO GARCIA ISMAEL ISAAC</t>
+    <t>2018010118</t>
+  </si>
+  <si>
+    <t>PACHECO PACHECO EDGAR</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>2018010008</t>
-  </si>
-  <si>
-    <t>MARCOS PEREZ LUIS REY</t>
+    <t>2018010289</t>
+  </si>
+  <si>
+    <t>AGUDO HERNANDEZ ITZEL</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>2018010020</t>
-  </si>
-  <si>
-    <t>RAMIREZ RUIZ NAYELI</t>
+    <t>2018010327</t>
+  </si>
+  <si>
+    <t>PALMA TERAN JESSICA ABIGAIL</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>2018010021</t>
-  </si>
-  <si>
-    <t>GARCIA PEREZ MARIA MAGDALENA</t>
+    <t>2018010454</t>
+  </si>
+  <si>
+    <t>HERNANDEZ DE LA PAZ RAUL</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>2018010030</t>
-  </si>
-  <si>
-    <t>MARTINEZ MARTINEZ WILFRIDO</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>2018010071</t>
-  </si>
-  <si>
-    <t>REYES  MOJICA DELFINO MISAEL</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>2018010072</t>
-  </si>
-  <si>
-    <t>GARCIA MARTINEZ DIEGO</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>2018010083</t>
-  </si>
-  <si>
-    <t>AGUILLON CHAVEZ JESUS</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>2018010118</t>
-  </si>
-  <si>
-    <t>PACHECO PACHECO EDGAR</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>2018010289</t>
-  </si>
-  <si>
-    <t>AGUDO HERNANDEZ ITZEL</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>2018010327</t>
-  </si>
-  <si>
-    <t>PALMA TERAN JESSICA ABIGAIL</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>2018010454</t>
-  </si>
-  <si>
-    <t>HERNANDEZ DE LA PAZ RAUL</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>2018010517</t>
   </si>
   <si>
     <t>HERNANDEZ VELASCO HECTOR</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>2018010520</t>
-  </si>
-  <si>
-    <t>ANTONIO JUAREZ RIGOBERTO</t>
-  </si>
-  <si>
     <t>TUTORIAS INDIVIDUALES</t>
   </si>
   <si>
@@ -217,9 +136,6 @@
   </si>
   <si>
     <t>901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOMEZ CRUZ GLORIA </t>
   </si>
 </sst>
 </file>
@@ -411,54 +327,54 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>64</v>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -466,8 +382,8 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -476,15 +392,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.2578125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="32.9296875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.00390625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.4375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="7.7890625" customWidth="true" bestFit="true"/>
   </cols>
@@ -653,159 +569,6 @@
         <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>